<commit_message>
dashboard2\dashboard\experiments2.R dashboard2\dashboard\reactive_server.R dashboard2\dashboard\views\Views.xlsx dashboard2\dashboard\views\create_view_page.R
</commit_message>
<xml_diff>
--- a/dashboard2/dashboard/views/Views.xlsx
+++ b/dashboard2/dashboard/views/Views.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -45,10 +45,19 @@
     <t xml:space="preserve">portal_code</t>
   </si>
   <si>
+    <t xml:space="preserve">admited_no, Available, course_id, no_of_seat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEMO1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admited_no, alloted_no, no_of_seat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FFFF</t>
+  </si>
+  <si>
     <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">admited_no, base_seat_yug</t>
   </si>
 </sst>
 </file>
@@ -400,7 +409,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
@@ -472,13 +481,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -486,13 +495,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>